<commit_message>
Add teams_members_permissions.xlsx - 2024-01-02 17:55:54
</commit_message>
<xml_diff>
--- a/teams_members_permissions.xlsx
+++ b/teams_members_permissions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,601 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>admin: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>maintain: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>admin: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>maintain: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>push: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>triage: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>admin: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>maintain: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>push: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>triage: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add teams_members_permissions.xlsx - 2024-01-02 18:07:27
</commit_message>
<xml_diff>
--- a/teams_members_permissions.xlsx
+++ b/teams_members_permissions.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>admin: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>maintain: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>push: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>triage: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>admin: False</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>maintain: False</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>push: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>triage: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>admin: True</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>maintain: True</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>push: True</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -672,7 +672,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>triage: True</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>admin: False</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>maintain: False</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>push: False</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>triage: False</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>admin: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>maintain: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>push: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>triage: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>admin: False</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>maintain: False</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>push: False</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -927,7 +927,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>triage: False</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>admin: False</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>maintain: False</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>push: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>triage: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>pull: True</t>
+          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add teams_members_permissions.xlsx - 2024-01-02 18:13:22
</commit_message>
<xml_diff>
--- a/teams_members_permissions.xlsx
+++ b/teams_members_permissions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
+          <t>admin: True</t>
         </is>
       </c>
     </row>
@@ -463,97 +463,573 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Team: firstgithubrepo-teamwrite</t>
+          <t>Team: firstgithubrepo-teamadmin</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>id: 543487077, node_id: R_kgDOIGT0ZQ, name: firstgithubrepo, full_name: github-gk-aks/firstgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/firstgithubrepo, description: First Repo for Migration to Github Enterprise, fork: False, url: https://api.github.com/repos/github-gk-aks/firstgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/firstgithubrepo/deployments, created_at: 2022-09-30T07:47:10Z, updated_at: 2023-12-05T14:07:44Z, pushed_at: 2023-12-29T14:00:44Z, git_url: git://github.com/github-gk-aks/firstgithubrepo.git, ssh_url: git@github.com:github-gk-aks/firstgithubrepo.git, clone_url: https://github.com/github-gk-aks/firstgithubrepo.git, svn_url: https://github.com/github-gk-aks/firstgithubrepo, homepage: , size: 117, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: True, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'other', 'name': 'Other', 'spdx_id': 'NOASSERTION', 'url': None, 'node_id': 'MDc6TGljZW5zZTA='}, allow_forking: True, topics: ['hello'], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
+          <t>maintain: True</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>github-gk-aks/secondgithubrepo</t>
+          <t>github-gk-aks/firstgithubrepo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Team: secondgithubrepo-teamadmin</t>
+          <t>Team: firstgithubrepo-teamadmin</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
+          <t>push: True</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>github-gk-aks/secondgithubrepo</t>
+          <t>github-gk-aks/firstgithubrepo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Team: secondgithubrepo-teamread</t>
+          <t>Team: firstgithubrepo-teamadmin</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>id: 714319907, node_id: R_kgDOKpOoIw, name: secondgithubrepo, full_name: github-gk-aks/secondgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/secondgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/secondgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/secondgithubrepo/deployments, created_at: 2023-11-04T15:05:43Z, updated_at: 2023-12-29T14:01:10Z, pushed_at: 2023-12-29T17:24:19Z, git_url: git://github.com/github-gk-aks/secondgithubrepo.git, ssh_url: git@github.com:github-gk-aks/secondgithubrepo.git, clone_url: https://github.com/github-gk-aks/secondgithubrepo.git, svn_url: https://github.com/github-gk-aks/secondgithubrepo, homepage: None, size: 51, stargazers_count: 0, watchers_count: 0, language: Python, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: None, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
+          <t>triage: True</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>github-gk-aks/thirdgithubrepo</t>
+          <t>github-gk-aks/firstgithubrepo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Team: thirdgithubrepo-teamadmin</t>
+          <t>Team: firstgithubrepo-teamadmin</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': True, 'maintain': True, 'push': True, 'triage': True, 'pull': True}, role_name: admin</t>
+          <t>pull: True</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>github-gk-aks/thirdgithubrepo</t>
+          <t>github-gk-aks/firstgithubrepo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team: thirdgithubrepo-teamread</t>
+          <t>Team: firstgithubrepo-teamwrite</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': False, 'triage': False, 'pull': True}, role_name: read</t>
+          <t>admin: False</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>github-gk-aks/thirdgithubrepo</t>
+          <t>github-gk-aks/firstgithubrepo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>github-gk-aks/firstgithubrepo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Team: firstgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>admin: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>maintain: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>push: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>triage: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>github-gk-aks/secondgithubrepo</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Team: secondgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>admin: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>maintain: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>push: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>triage: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>Team: thirdgithubrepo-teamwrite</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>id: 714931038, node_id: R_kgDOKpz7Xg, name: thirdgithubrepo, full_name: github-gk-aks/thirdgithubrepo, private: False, owner: {'login': 'github-gk-aks', 'id': 114729278, 'node_id': 'O_kgDOBtahPg', 'avatar_url': 'https://avatars.githubusercontent.com/u/114729278?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/github-gk-aks', 'html_url': 'https://github.com/github-gk-aks', 'followers_url': 'https://api.github.com/users/github-gk-aks/followers', 'following_url': 'https://api.github.com/users/github-gk-aks/following{/other_user}', 'gists_url': 'https://api.github.com/users/github-gk-aks/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/github-gk-aks/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/github-gk-aks/subscriptions', 'organizations_url': 'https://api.github.com/users/github-gk-aks/orgs', 'repos_url': 'https://api.github.com/users/github-gk-aks/repos', 'events_url': 'https://api.github.com/users/github-gk-aks/events{/privacy}', 'received_events_url': 'https://api.github.com/users/github-gk-aks/received_events', 'type': 'Organization', 'site_admin': False}, html_url: https://github.com/github-gk-aks/thirdgithubrepo, description: Repo for testing out the Github Migration process, fork: False, url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo, forks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/forks, keys_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/keys{/key_id}, collaborators_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/collaborators{/collaborator}, teams_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/teams, hooks_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/hooks, issue_events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/events{/number}, events_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/events, assignees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/assignees{/user}, branches_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/branches{/branch}, tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/tags, blobs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/blobs{/sha}, git_tags_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/tags{/sha}, git_refs_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/refs{/sha}, trees_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/trees{/sha}, statuses_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/statuses/{sha}, languages_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/languages, stargazers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/stargazers, contributors_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contributors, subscribers_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscribers, subscription_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/subscription, commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/commits{/sha}, git_commits_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/git/commits{/sha}, comments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/comments{/number}, issue_comment_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues/comments{/number}, contents_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/contents/{+path}, compare_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/compare/{base}...{head}, merges_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/merges, archive_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/{archive_format}{/ref}, downloads_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/downloads, issues_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/issues{/number}, pulls_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/pulls{/number}, milestones_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/milestones{/number}, notifications_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/notifications{?since,all,participating}, labels_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/labels{/name}, releases_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/releases{/id}, deployments_url: https://api.github.com/repos/github-gk-aks/thirdgithubrepo/deployments, created_at: 2023-11-06T06:20:21Z, updated_at: 2023-11-14T12:16:50Z, pushed_at: 2023-12-04T15:39:05Z, git_url: git://github.com/github-gk-aks/thirdgithubrepo.git, ssh_url: git@github.com:github-gk-aks/thirdgithubrepo.git, clone_url: https://github.com/github-gk-aks/thirdgithubrepo.git, svn_url: https://github.com/github-gk-aks/thirdgithubrepo, homepage: None, size: 33, stargazers_count: 0, watchers_count: 0, language: None, has_issues: True, has_projects: False, has_downloads: True, has_wiki: False, has_pages: False, forks_count: 0, mirror_url: None, archived: False, disabled: False, open_issues_count: 0, license: {'key': 'mit', 'name': 'MIT License', 'spdx_id': 'MIT', 'url': 'https://api.github.com/licenses/mit', 'node_id': 'MDc6TGljZW5zZTEz'}, allow_forking: True, topics: [], visibility: public, forks: 0, open_issues: 0, watchers: 0, default_branch: main, temp_clone_token: , allow_squash_merge: True, allow_merge_commit: True, allow_rebase_merge: True, allow_auto_merge: False, delete_branch_on_merge: True, permissions: {'admin': False, 'maintain': False, 'push': True, 'triage': True, 'pull': True}, role_name: write</t>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>admin: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>maintain: False</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>push: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>triage: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamwrite</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>pull: True</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add teams_members_permissions.xlsx - 2024-01-04 08:49:57
</commit_message>
<xml_diff>
--- a/teams_members_permissions.xlsx
+++ b/teams_members_permissions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,17 +475,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>github-gk-aks/secondgithubrepo</t>
+          <t>github-gk-aks/firstgithubrepo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Team: secondgithubrepo-teamadmin</t>
+          <t>User: gauravkhanna3007</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>admin: True, maintain: True, push: True, triage: True, pull: True</t>
+          <t>Permission: admin</t>
         </is>
       </c>
     </row>
@@ -497,46 +497,46 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Team: secondgithubrepo-teamread</t>
+          <t>Team: secondgithubrepo-teamadmin</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>admin: False, maintain: False, push: False, triage: False, pull: True</t>
+          <t>admin: True, maintain: True, push: True, triage: True, pull: True</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>github-gk-aks/thirdgithubrepo</t>
+          <t>github-gk-aks/secondgithubrepo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Team: thirdgithubrepo-teamadmin</t>
+          <t>Team: secondgithubrepo-teamread</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>admin: True, maintain: True, push: True, triage: True, pull: True</t>
+          <t>admin: False, maintain: False, push: False, triage: False, pull: True</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>github-gk-aks/thirdgithubrepo</t>
+          <t>github-gk-aks/secondgithubrepo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team: thirdgithubrepo-teamread</t>
+          <t>User: gauravkhanna3007</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>admin: False, maintain: False, push: False, triage: False, pull: True</t>
+          <t>Permission: admin</t>
         </is>
       </c>
     </row>
@@ -548,12 +548,80 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Team: thirdgithubrepo-teamadmin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>admin: True, maintain: True, push: True, triage: True, pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Team: thirdgithubrepo-teamread</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>admin: False, maintain: False, push: False, triage: False, pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Team: thirdgithubrepo-teamwrite</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>admin: False, maintain: False, push: True, triage: True, pull: True</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>User: arvindsi1973</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Permission: read</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>github-gk-aks/thirdgithubrepo</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>User: srinu220kv</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Permission: read</t>
         </is>
       </c>
     </row>

</xml_diff>